<commit_message>
Updates in code and database
Updates in code and database
</commit_message>
<xml_diff>
--- a/Codes/SOE+Prices+MP+Datos/Datos/DataCOL.xlsx
+++ b/Codes/SOE+Prices+MP+Datos/Datos/DataCOL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarincong/Documents/Git Repos/Cursos_Banrep/Codes/SOE+Prices+MP+Datos/Datos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fredy\Documents\GIT repos\Courses_BanRep\Codes\SOE+Prices+MP+Datos\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCC9128C-EC92-0D46-898B-9BE4BBC364AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{706C7AC4-2CBC-49D9-88C8-1A865E6EC93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{3B812F19-A572-41B0-90ED-022F2B941229}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{3B812F19-A572-41B0-90ED-022F2B941229}"/>
   </bookViews>
   <sheets>
     <sheet name="Data_Forecast" sheetId="2" r:id="rId1"/>
@@ -188,7 +188,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -491,27 +491,27 @@
       <selection pane="bottomLeft" activeCell="K103" sqref="K103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
     <col min="14" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="9.6640625" customWidth="1"/>
-    <col min="23" max="24" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.7109375" customWidth="1"/>
+    <col min="23" max="24" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -576,7 +576,7 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>36586</v>
       </c>
@@ -632,7 +632,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>36678</v>
       </c>
@@ -697,7 +697,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>36770</v>
       </c>
@@ -769,7 +769,7 @@
       <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>36861</v>
       </c>
@@ -834,7 +834,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>36951</v>
       </c>
@@ -899,7 +899,7 @@
         <v>0.11888888888888889</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>37043</v>
       </c>
@@ -964,7 +964,7 @@
         <v>0.115</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>37135</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>0.10592391304347826</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>37226</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>8.983695652173912E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>37316</v>
       </c>
@@ -1159,7 +1159,7 @@
         <v>7.9944444444444443E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>37408</v>
       </c>
@@ -1224,7 +1224,7 @@
         <v>6.0961538461538456E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>37500</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>5.2499999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>37591</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>5.2499999999999998E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>37681</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>6.0388888888888888E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>37773</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>6.9423076923076921E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>37865</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>7.2499999999999995E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>37956</v>
       </c>
@@ -1614,7 +1614,7 @@
         <v>7.2499999999999995E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>38047</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>7.12087912087912E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>38139</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>6.7500000000000004E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>38231</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>6.7500000000000004E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>38322</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>6.7173913043478264E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>38412</v>
       </c>
@@ -1939,7 +1939,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>38504</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>38596</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>6.4347826086956522E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>38687</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>38777</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>38869</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>6.1923076923076928E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>38961</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>6.6086956521739126E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>39052</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>7.2065217391304351E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>39142</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>7.7833333333333338E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>39234</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>8.5576923076923078E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>39326</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>9.1711956521739121E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>39417</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>9.3478260869565219E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>39508</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>9.5989010989010984E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>39600</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>9.7500000000000003E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>39692</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>9.9266304347826087E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>39783</v>
       </c>
@@ -2914,7 +2914,7 @@
         <v>9.945652173913043E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>39873</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>8.7555555555555567E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>39965</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>5.9890109890109892E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>40057</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>4.4836956521739128E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40148</v>
       </c>
@@ -3174,7 +3174,7 @@
         <v>3.7934782608695657E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40238</v>
       </c>
@@ -3239,7 +3239,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>40330</v>
       </c>
@@ -3304,7 +3304,7 @@
         <v>3.1758241758241754E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>40422</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>40513</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>40603</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>3.1166666666666665E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>40695</v>
       </c>
@@ -3564,7 +3564,7 @@
         <v>3.7802197802197804E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>40787</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>4.4157608695652176E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>40878</v>
       </c>
@@ -3694,7 +3694,7 @@
         <v>4.5923913043478259E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>40969</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>5.0109890109890108E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>41061</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>5.2499999999999998E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>41153</v>
       </c>
@@ -3889,7 +3889,7 @@
         <v>4.9836956521739133E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>41244</v>
       </c>
@@ -3954,7 +3954,7 @@
         <v>4.6304347826086951E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>41334</v>
       </c>
@@ -4019,7 +4019,7 @@
         <v>3.9472222222222221E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>41426</v>
       </c>
@@ -4084,7 +4084,7 @@
         <v>3.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>41518</v>
       </c>
@@ -4149,7 +4149,7 @@
         <v>3.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>41609</v>
       </c>
@@ -4214,7 +4214,7 @@
         <v>3.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>41699</v>
       </c>
@@ -4279,7 +4279,7 @@
         <v>3.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>41791</v>
       </c>
@@ -4344,7 +4344,7 @@
         <v>3.5219780219780221E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>41883</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>4.2472826086956524E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>41974</v>
       </c>
@@ -4474,7 +4474,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>42064</v>
       </c>
@@ -4539,7 +4539,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>42156</v>
       </c>
@@ -4604,7 +4604,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>42248</v>
       </c>
@@ -4669,7 +4669,7 @@
         <v>4.5081521739130437E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>42339</v>
       </c>
@@ -4734,7 +4734,7 @@
         <v>5.1874999999999998E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>42430</v>
       </c>
@@ -4799,7 +4799,7 @@
         <v>6.0494505494505496E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>42522</v>
       </c>
@@ -4864,7 +4864,7 @@
         <v>6.9368131868131871E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>42614</v>
       </c>
@@ -4929,7 +4929,7 @@
         <v>7.6657608695652177E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>42705</v>
       </c>
@@ -4994,7 +4994,7 @@
         <v>7.714673913043478E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>42795</v>
       </c>
@@ -5059,7 +5059,7 @@
         <v>7.3944444444444452E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>42887</v>
       </c>
@@ -5124,7 +5124,7 @@
         <v>6.5824175824175823E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>42979</v>
       </c>
@@ -5189,7 +5189,7 @@
         <v>5.5081521739130439E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>43070</v>
       </c>
@@ -5254,7 +5254,7 @@
         <v>4.9836956521739133E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>43160</v>
       </c>
@@ -5319,7 +5319,7 @@
         <v>4.5805555555555558E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>43252</v>
       </c>
@@ -5384,7 +5384,7 @@
         <v>4.3296703296703293E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>43344</v>
       </c>
@@ -5449,7 +5449,7 @@
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>43435</v>
       </c>
@@ -5514,7 +5514,7 @@
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>43525</v>
       </c>
@@ -5579,7 +5579,7 @@
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>43617</v>
       </c>
@@ -5644,7 +5644,7 @@
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>43709</v>
       </c>
@@ -5709,7 +5709,7 @@
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>43800</v>
       </c>
@@ -5774,7 +5774,7 @@
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>43891</v>
       </c>
@@ -5839,7 +5839,7 @@
         <v>4.2390109890109891E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>43983</v>
       </c>
@@ -5904,7 +5904,7 @@
         <v>3.2664835164835163E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>44075</v>
       </c>
@@ -5969,7 +5969,7 @@
         <v>2.2499999999999999E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>44166</v>
       </c>
@@ -6034,7 +6034,7 @@
         <v>1.7500000000000002E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>44256</v>
       </c>
@@ -6099,7 +6099,7 @@
         <v>1.7500000000000002E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>44348</v>
       </c>
@@ -6164,7 +6164,7 @@
         <v>1.7500000000000002E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>44440</v>
       </c>
@@ -6229,7 +6229,7 @@
         <v>1.7500000000000002E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>44531</v>
       </c>
@@ -6294,7 +6294,7 @@
         <v>2.391304347826087E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>44621</v>
       </c>
@@ -6359,7 +6359,7 @@
         <v>3.6666666666666667E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>44713</v>
       </c>
@@ -6424,7 +6424,7 @@
         <v>5.6593406593406594E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>44805</v>
       </c>
@@ -6489,7 +6489,7 @@
         <v>8.5054347826086951E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="6">
         <v>44896</v>
       </c>
@@ -6554,7 +6554,7 @@
         <v>0.10815217391304348</v>
       </c>
     </row>
-    <row r="94" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="10">
         <v>44986</v>
       </c>
@@ -6586,7 +6586,7 @@
       <c r="S94" s="11"/>
       <c r="T94" s="11"/>
     </row>
-    <row r="95" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="10">
         <v>45078</v>
       </c>
@@ -6618,7 +6618,7 @@
       <c r="S95" s="11"/>
       <c r="T95" s="11"/>
     </row>
-    <row r="96" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="10">
         <v>45170</v>
       </c>
@@ -6648,7 +6648,7 @@
       <c r="S96" s="11"/>
       <c r="T96" s="11"/>
     </row>
-    <row r="97" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="10">
         <v>45261</v>
       </c>
@@ -6678,7 +6678,7 @@
       <c r="S97" s="11"/>
       <c r="T97" s="11"/>
     </row>
-    <row r="98" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="10">
         <v>45352</v>
       </c>
@@ -6708,7 +6708,7 @@
       <c r="S98" s="11"/>
       <c r="T98" s="11"/>
     </row>
-    <row r="99" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="10">
         <v>45444</v>
       </c>
@@ -6738,7 +6738,7 @@
       <c r="S99" s="11"/>
       <c r="T99" s="11"/>
     </row>
-    <row r="100" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="10">
         <v>45536</v>
       </c>
@@ -6768,7 +6768,7 @@
       <c r="S100" s="11"/>
       <c r="T100" s="11"/>
     </row>
-    <row r="101" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="10">
         <v>45627</v>
       </c>
@@ -6798,7 +6798,7 @@
       <c r="S101" s="11"/>
       <c r="T101" s="11"/>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>45717</v>
       </c>
@@ -6822,7 +6822,7 @@
       <c r="S102" s="8"/>
       <c r="T102" s="8"/>
     </row>
-    <row r="103" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="6">
         <v>45809</v>
       </c>
@@ -6846,123 +6846,123 @@
       <c r="S103" s="9"/>
       <c r="T103" s="9"/>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>45901</v>
       </c>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>45992</v>
       </c>
       <c r="F105" s="8"/>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>46082</v>
       </c>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>46174</v>
       </c>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>46266</v>
       </c>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>46357</v>
       </c>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>46447</v>
       </c>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>46539</v>
       </c>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>46631</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>46722</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>46813</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="6">
         <v>46905</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>46997</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>47088</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>47178</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>47270</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>47362</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>47453</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>47543</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>47635</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>47727</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>47818</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>47908</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="6">
         <v>48000</v>
       </c>
@@ -6977,32 +6977,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC43C700-5E37-433E-91EB-5805D755A630}">
   <dimension ref="A1:AC127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="268" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
     <col min="14" max="19" width="11" customWidth="1"/>
-    <col min="20" max="20" width="9.6640625" customWidth="1"/>
-    <col min="23" max="24" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.7109375" customWidth="1"/>
+    <col min="23" max="24" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -7067,7 +7067,7 @@
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>36586</v>
       </c>
@@ -7123,7 +7123,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>36678</v>
       </c>
@@ -7188,7 +7188,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>36770</v>
       </c>
@@ -7260,7 +7260,7 @@
       <c r="AB4" s="2"/>
       <c r="AC4" s="2"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>36861</v>
       </c>
@@ -7325,7 +7325,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>36951</v>
       </c>
@@ -7390,7 +7390,7 @@
         <v>0.11888888888888889</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>37043</v>
       </c>
@@ -7455,7 +7455,7 @@
         <v>0.115</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>37135</v>
       </c>
@@ -7520,7 +7520,7 @@
         <v>0.10592391304347826</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>37226</v>
       </c>
@@ -7585,7 +7585,7 @@
         <v>8.983695652173912E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>37316</v>
       </c>
@@ -7650,7 +7650,7 @@
         <v>7.9944444444444443E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>37408</v>
       </c>
@@ -7715,7 +7715,7 @@
         <v>6.0961538461538456E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>37500</v>
       </c>
@@ -7780,7 +7780,7 @@
         <v>5.2499999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>37591</v>
       </c>
@@ -7845,7 +7845,7 @@
         <v>5.2499999999999998E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>37681</v>
       </c>
@@ -7910,7 +7910,7 @@
         <v>6.0388888888888888E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>37773</v>
       </c>
@@ -7975,7 +7975,7 @@
         <v>6.9423076923076921E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>37865</v>
       </c>
@@ -8040,7 +8040,7 @@
         <v>7.2499999999999995E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>37956</v>
       </c>
@@ -8105,7 +8105,7 @@
         <v>7.2499999999999995E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>38047</v>
       </c>
@@ -8170,7 +8170,7 @@
         <v>7.12087912087912E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>38139</v>
       </c>
@@ -8235,7 +8235,7 @@
         <v>6.7500000000000004E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>38231</v>
       </c>
@@ -8300,7 +8300,7 @@
         <v>6.7500000000000004E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>38322</v>
       </c>
@@ -8365,7 +8365,7 @@
         <v>6.7173913043478264E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>38412</v>
       </c>
@@ -8430,7 +8430,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>38504</v>
       </c>
@@ -8495,7 +8495,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>38596</v>
       </c>
@@ -8560,7 +8560,7 @@
         <v>6.4347826086956522E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>38687</v>
       </c>
@@ -8625,7 +8625,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>38777</v>
       </c>
@@ -8690,7 +8690,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>38869</v>
       </c>
@@ -8755,7 +8755,7 @@
         <v>6.1923076923076928E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>38961</v>
       </c>
@@ -8820,7 +8820,7 @@
         <v>6.6086956521739126E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>39052</v>
       </c>
@@ -8885,7 +8885,7 @@
         <v>7.2065217391304351E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>39142</v>
       </c>
@@ -8950,7 +8950,7 @@
         <v>7.7833333333333338E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>39234</v>
       </c>
@@ -9015,7 +9015,7 @@
         <v>8.5576923076923078E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>39326</v>
       </c>
@@ -9080,7 +9080,7 @@
         <v>9.1711956521739121E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>39417</v>
       </c>
@@ -9145,7 +9145,7 @@
         <v>9.3478260869565219E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>39508</v>
       </c>
@@ -9210,7 +9210,7 @@
         <v>9.5989010989010984E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>39600</v>
       </c>
@@ -9275,7 +9275,7 @@
         <v>9.7500000000000003E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>39692</v>
       </c>
@@ -9340,7 +9340,7 @@
         <v>9.9266304347826087E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>39783</v>
       </c>
@@ -9405,7 +9405,7 @@
         <v>9.945652173913043E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>39873</v>
       </c>
@@ -9470,7 +9470,7 @@
         <v>8.7555555555555567E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>39965</v>
       </c>
@@ -9535,7 +9535,7 @@
         <v>5.9890109890109892E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>40057</v>
       </c>
@@ -9600,7 +9600,7 @@
         <v>4.4836956521739128E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40148</v>
       </c>
@@ -9665,7 +9665,7 @@
         <v>3.7934782608695657E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40238</v>
       </c>
@@ -9730,7 +9730,7 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>40330</v>
       </c>
@@ -9795,7 +9795,7 @@
         <v>3.1758241758241754E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>40422</v>
       </c>
@@ -9860,7 +9860,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>40513</v>
       </c>
@@ -9925,7 +9925,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>40603</v>
       </c>
@@ -9990,7 +9990,7 @@
         <v>3.1166666666666665E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>40695</v>
       </c>
@@ -10055,7 +10055,7 @@
         <v>3.7802197802197804E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>40787</v>
       </c>
@@ -10120,7 +10120,7 @@
         <v>4.4157608695652176E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>40878</v>
       </c>
@@ -10185,7 +10185,7 @@
         <v>4.5923913043478259E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>40969</v>
       </c>
@@ -10250,7 +10250,7 @@
         <v>5.0109890109890108E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>41061</v>
       </c>
@@ -10315,7 +10315,7 @@
         <v>5.2499999999999998E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>41153</v>
       </c>
@@ -10380,7 +10380,7 @@
         <v>4.9836956521739133E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>41244</v>
       </c>
@@ -10445,7 +10445,7 @@
         <v>4.6304347826086951E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>41334</v>
       </c>
@@ -10510,7 +10510,7 @@
         <v>3.9472222222222221E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>41426</v>
       </c>
@@ -10575,7 +10575,7 @@
         <v>3.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>41518</v>
       </c>
@@ -10640,7 +10640,7 @@
         <v>3.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>41609</v>
       </c>
@@ -10705,7 +10705,7 @@
         <v>3.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>41699</v>
       </c>
@@ -10770,7 +10770,7 @@
         <v>3.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>41791</v>
       </c>
@@ -10835,7 +10835,7 @@
         <v>3.5219780219780221E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>41883</v>
       </c>
@@ -10900,7 +10900,7 @@
         <v>4.2472826086956524E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>41974</v>
       </c>
@@ -10965,7 +10965,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>42064</v>
       </c>
@@ -11030,7 +11030,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>42156</v>
       </c>
@@ -11095,7 +11095,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>42248</v>
       </c>
@@ -11160,7 +11160,7 @@
         <v>4.5081521739130437E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>42339</v>
       </c>
@@ -11225,7 +11225,7 @@
         <v>5.1874999999999998E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>42430</v>
       </c>
@@ -11290,7 +11290,7 @@
         <v>6.0494505494505496E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>42522</v>
       </c>
@@ -11355,7 +11355,7 @@
         <v>6.9368131868131871E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>42614</v>
       </c>
@@ -11420,7 +11420,7 @@
         <v>7.6657608695652177E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>42705</v>
       </c>
@@ -11485,7 +11485,7 @@
         <v>7.714673913043478E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>42795</v>
       </c>
@@ -11550,7 +11550,7 @@
         <v>7.3944444444444452E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>42887</v>
       </c>
@@ -11615,7 +11615,7 @@
         <v>6.5824175824175823E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>42979</v>
       </c>
@@ -11680,7 +11680,7 @@
         <v>5.5081521739130439E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>43070</v>
       </c>
@@ -11745,7 +11745,7 @@
         <v>4.9836956521739133E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>43160</v>
       </c>
@@ -11810,7 +11810,7 @@
         <v>4.5805555555555558E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>43252</v>
       </c>
@@ -11875,7 +11875,7 @@
         <v>4.3296703296703293E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>43344</v>
       </c>
@@ -11940,7 +11940,7 @@
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>43435</v>
       </c>
@@ -12005,7 +12005,7 @@
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>43525</v>
       </c>
@@ -12070,7 +12070,7 @@
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>43617</v>
       </c>
@@ -12135,7 +12135,7 @@
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>43709</v>
       </c>
@@ -12200,7 +12200,7 @@
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>43800</v>
       </c>
@@ -12265,7 +12265,7 @@
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>43891</v>
       </c>
@@ -12330,7 +12330,7 @@
         <v>4.2390109890109891E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>43983</v>
       </c>
@@ -12395,7 +12395,7 @@
         <v>3.2664835164835163E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>44075</v>
       </c>
@@ -12460,7 +12460,7 @@
         <v>2.2499999999999999E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>44166</v>
       </c>
@@ -12525,7 +12525,7 @@
         <v>1.7500000000000002E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>44256</v>
       </c>
@@ -12590,7 +12590,7 @@
         <v>1.7500000000000002E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>44348</v>
       </c>
@@ -12655,7 +12655,7 @@
         <v>1.7500000000000002E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>44440</v>
       </c>
@@ -12720,7 +12720,7 @@
         <v>1.7500000000000002E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>44531</v>
       </c>
@@ -12785,7 +12785,7 @@
         <v>2.391304347826087E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>44621</v>
       </c>
@@ -12850,7 +12850,7 @@
         <v>3.6666666666666667E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>44713</v>
       </c>
@@ -12915,7 +12915,7 @@
         <v>5.6593406593406594E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>44805</v>
       </c>
@@ -12980,7 +12980,7 @@
         <v>8.5054347826086951E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>44896</v>
       </c>
@@ -13045,7 +13045,7 @@
         <v>0.10815217391304348</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>44986</v>
       </c>
@@ -13110,7 +13110,7 @@
         <v>0.12511111111111112</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>45078</v>
       </c>
@@ -13175,7 +13175,7 @@
         <v>0.13164835164835165</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>45170</v>
       </c>
@@ -13240,7 +13240,7 @@
         <v>0.13250000000000001</v>
       </c>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>45261</v>
       </c>
@@ -13305,7 +13305,7 @@
         <v>0.13217391304347825</v>
       </c>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>45352</v>
       </c>
@@ -13370,7 +13370,7 @@
         <v>0.12802197802197804</v>
       </c>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>45444</v>
       </c>
@@ -13435,7 +13435,7 @@
         <v>0.1192032967032967</v>
       </c>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>45536</v>
       </c>
@@ -13500,7 +13500,7 @@
         <v>0.10923913043478262</v>
       </c>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>45627</v>
       </c>
@@ -13565,7 +13565,7 @@
         <v>9.8940217391304361E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>45717</v>
       </c>
@@ -13630,7 +13630,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:20" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="6">
         <v>45809</v>
       </c>
@@ -13677,123 +13677,123 @@
         <v>9.3351648351648359E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>45901</v>
       </c>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>45992</v>
       </c>
       <c r="F105" s="8"/>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>46082</v>
       </c>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>46174</v>
       </c>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>46266</v>
       </c>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>46357</v>
       </c>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>46447</v>
       </c>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>46539</v>
       </c>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>46631</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>46722</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>46813</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="6">
         <v>46905</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>46997</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>47088</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>47178</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>47270</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>47362</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>47453</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>47543</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>47635</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>47727</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>47818</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>47908</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="6">
         <v>48000</v>
       </c>

</xml_diff>